<commit_message>
bug fixes and reduce average scores to 0-1
</commit_message>
<xml_diff>
--- a/ConfigSheet.xlsx
+++ b/ConfigSheet.xlsx
@@ -465,7 +465,7 @@
         </is>
       </c>
       <c r="D2" t="n">
-        <v>5.299</v>
+        <v>0.4913160583263677</v>
       </c>
     </row>
     <row r="3">
@@ -483,7 +483,7 @@
         </is>
       </c>
       <c r="D3" t="n">
-        <v>4.621</v>
+        <v>0.4292746354602025</v>
       </c>
     </row>
     <row r="4">
@@ -501,7 +501,7 @@
         </is>
       </c>
       <c r="D4" t="n">
-        <v>4.486</v>
+        <v>0.4168292003343551</v>
       </c>
     </row>
     <row r="5">
@@ -519,7 +519,7 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>5.367</v>
+        <v>0.4987461688492617</v>
       </c>
     </row>
     <row r="6">
@@ -537,7 +537,7 @@
         </is>
       </c>
       <c r="D6" t="n">
-        <v>4.699</v>
+        <v>0.4359617349308071</v>
       </c>
     </row>
     <row r="7">
@@ -555,7 +555,7 @@
         </is>
       </c>
       <c r="D7" t="n">
-        <v>4.817320169391373</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -573,7 +573,7 @@
         </is>
       </c>
       <c r="D8" t="n">
-        <v>4.269</v>
+        <v>0.4531438655149995</v>
       </c>
     </row>
     <row r="9">
@@ -591,7 +591,7 @@
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1.089</v>
+        <v>0.1717284294603882</v>
       </c>
     </row>
     <row r="10">
@@ -609,7 +609,7 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>0.53</v>
+        <v>0</v>
       </c>
     </row>
     <row r="11">
@@ -627,7 +627,7 @@
         </is>
       </c>
       <c r="D11" t="n">
-        <v>4.121</v>
+        <v>0.3434568589207765</v>
       </c>
     </row>
     <row r="12">
@@ -645,7 +645,7 @@
         </is>
       </c>
       <c r="D12" t="n">
-        <v>3.192</v>
+        <v>0.4520293489365654</v>
       </c>
     </row>
     <row r="13">
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="D13" t="n">
-        <v>3.254</v>
+        <v>0.4372620042723136</v>
       </c>
     </row>
     <row r="14">
@@ -681,7 +681,7 @@
         </is>
       </c>
       <c r="D14" t="n">
-        <v>3.997</v>
+        <v>0.284944738552986</v>
       </c>
     </row>
     <row r="15">
@@ -699,7 +699,7 @@
         </is>
       </c>
       <c r="D15" t="n">
-        <v>5.237</v>
+        <v>0.6878424816569146</v>
       </c>
     </row>
     <row r="16">
@@ -717,7 +717,7 @@
         </is>
       </c>
       <c r="D16" t="n">
-        <v>0.84</v>
+        <v>0</v>
       </c>
     </row>
     <row r="17">
@@ -735,7 +735,7 @@
         </is>
       </c>
       <c r="D17" t="n">
-        <v>3.328</v>
+        <v>0.09928485186217145</v>
       </c>
     </row>
     <row r="18">
@@ -753,7 +753,7 @@
         </is>
       </c>
       <c r="D18" t="n">
-        <v>3.51742429676118</v>
+        <v>0</v>
       </c>
     </row>
     <row r="19">
@@ -771,7 +771,7 @@
         </is>
       </c>
       <c r="D19" t="n">
-        <v>2.843</v>
+        <v>0.3240456951797158</v>
       </c>
     </row>
     <row r="20">
@@ -789,7 +789,7 @@
         </is>
       </c>
       <c r="D20" t="n">
-        <v>3.898</v>
+        <v>0.3404848147116188</v>
       </c>
     </row>
     <row r="21">
@@ -807,7 +807,7 @@
         </is>
       </c>
       <c r="D21" t="n">
-        <v>2.65</v>
+        <v>0.1021640196897929</v>
       </c>
     </row>
     <row r="22">
@@ -825,7 +825,7 @@
         </is>
       </c>
       <c r="D22" t="n">
-        <v>7.309</v>
+        <v>0.9145537289867187</v>
       </c>
     </row>
     <row r="23">
@@ -861,7 +861,7 @@
         </is>
       </c>
       <c r="D24" t="n">
-        <v>2.890078983651763</v>
+        <v>0</v>
       </c>
     </row>
     <row r="25">
@@ -879,7 +879,7 @@
         </is>
       </c>
       <c r="D25" t="n">
-        <v>3.611</v>
+        <v>0.2679483607318659</v>
       </c>
     </row>
     <row r="26">
@@ -897,7 +897,7 @@
         </is>
       </c>
       <c r="D26" t="n">
-        <v>2.134</v>
+        <v>0.1563109501253831</v>
       </c>
     </row>
     <row r="27">
@@ -915,7 +915,7 @@
         </is>
       </c>
       <c r="D27" t="n">
-        <v>2.579</v>
+        <v>0.1935543791213895</v>
       </c>
     </row>
     <row r="28">
@@ -933,7 +933,7 @@
         </is>
       </c>
       <c r="D28" t="n">
-        <v>4.013</v>
+        <v>0.375499210550757</v>
       </c>
     </row>
     <row r="29">
@@ -951,7 +951,7 @@
         </is>
       </c>
       <c r="D29" t="n">
-        <v>1.518</v>
+        <v>0.2356273799572769</v>
       </c>
     </row>
     <row r="30">
@@ -969,7 +969,7 @@
         </is>
       </c>
       <c r="D30" t="n">
-        <v>3.884</v>
+        <v>0.3435497353023126</v>
       </c>
     </row>
     <row r="31">
@@ -987,7 +987,7 @@
         </is>
       </c>
       <c r="D31" t="n">
-        <v>7.511</v>
+        <v>0.6271013281322559</v>
       </c>
     </row>
     <row r="32">
@@ -1005,7 +1005,7 @@
         </is>
       </c>
       <c r="D32" t="n">
-        <v>3.672945681554898</v>
+        <v>0</v>
       </c>
     </row>
     <row r="33">
@@ -1023,7 +1023,7 @@
         </is>
       </c>
       <c r="D33" t="n">
-        <v>4.203</v>
+        <v>0.3439212408284573</v>
       </c>
     </row>
     <row r="34">
@@ -1041,7 +1041,7 @@
         </is>
       </c>
       <c r="D34" t="n">
-        <v>4.355</v>
+        <v>0.3881303984396768</v>
       </c>
     </row>
     <row r="35">
@@ -1059,7 +1059,7 @@
         </is>
       </c>
       <c r="D35" t="n">
-        <v>1.736</v>
+        <v>0.230890684498932</v>
       </c>
     </row>
     <row r="36">
@@ -1077,7 +1077,7 @@
         </is>
       </c>
       <c r="D36" t="n">
-        <v>4.244</v>
+        <v>0.3908238135042259</v>
       </c>
     </row>
     <row r="37">
@@ -1095,7 +1095,7 @@
         </is>
       </c>
       <c r="D37" t="n">
-        <v>3.283</v>
+        <v>0.3089068449893193</v>
       </c>
     </row>
     <row r="38">
@@ -1113,7 +1113,7 @@
         </is>
       </c>
       <c r="D38" t="n">
-        <v>0.8026257632460114</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39">
@@ -1131,7 +1131,7 @@
         </is>
       </c>
       <c r="D39" t="n">
-        <v>0.469</v>
+        <v>0.07820191325345964</v>
       </c>
     </row>
     <row r="40">
@@ -1149,7 +1149,7 @@
         </is>
       </c>
       <c r="D40" t="n">
-        <v>3.048</v>
+        <v>0.3238599424166435</v>
       </c>
     </row>
     <row r="41">
@@ -1167,7 +1167,7 @@
         </is>
       </c>
       <c r="D41" t="n">
-        <v>0.9379999999999999</v>
+        <v>0</v>
       </c>
     </row>
     <row r="42">
@@ -1185,7 +1185,7 @@
         </is>
       </c>
       <c r="D42" t="n">
-        <v>4.215089915304314</v>
+        <v>0</v>
       </c>
     </row>
     <row r="43">
@@ -1203,7 +1203,7 @@
         </is>
       </c>
       <c r="D43" t="n">
-        <v>3.025</v>
+        <v>0.394538868765673</v>
       </c>
     </row>
     <row r="44">
@@ -1221,7 +1221,7 @@
         </is>
       </c>
       <c r="D44" t="n">
-        <v>0.399</v>
+        <v>0</v>
       </c>
     </row>
     <row r="45">
@@ -1239,7 +1239,7 @@
         </is>
       </c>
       <c r="D45" t="n">
-        <v>5.088</v>
+        <v>0.4280672425002322</v>
       </c>
     </row>
     <row r="46">
@@ -1293,7 +1293,7 @@
         </is>
       </c>
       <c r="D48" t="n">
-        <v>3.411942288753201</v>
+        <v>0</v>
       </c>
     </row>
     <row r="49">
@@ -1311,7 +1311,7 @@
         </is>
       </c>
       <c r="D49" t="n">
-        <v>4.689</v>
+        <v>0.3163369555122132</v>
       </c>
     </row>
     <row r="50">
@@ -1329,7 +1329,7 @@
         </is>
       </c>
       <c r="D50" t="n">
-        <v>0.797</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51">
@@ -1347,7 +1347,7 @@
         </is>
       </c>
       <c r="D51" t="n">
-        <v>0.352</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52">
@@ -1365,7 +1365,7 @@
         </is>
       </c>
       <c r="D52" t="n">
-        <v>4.455668898956077</v>
+        <v>0</v>
       </c>
     </row>
     <row r="53">
@@ -1383,7 +1383,7 @@
         </is>
       </c>
       <c r="D53" t="n">
-        <v>4.291</v>
+        <v>0.413114145072908</v>
       </c>
     </row>
     <row r="54">
@@ -1401,7 +1401,7 @@
         </is>
       </c>
       <c r="D54" t="n">
-        <v>3.892</v>
+        <v>0.1227825763908238</v>
       </c>
     </row>
     <row r="55">
@@ -1419,7 +1419,7 @@
         </is>
       </c>
       <c r="D55" t="n">
-        <v>0.516</v>
+        <v>0</v>
       </c>
     </row>
     <row r="56">
@@ -1437,7 +1437,7 @@
         </is>
       </c>
       <c r="D56" t="n">
-        <v>3.387</v>
+        <v>0.2204885297668803</v>
       </c>
     </row>
     <row r="57">
@@ -1455,7 +1455,7 @@
         </is>
       </c>
       <c r="D57" t="n">
-        <v>2.952</v>
+        <v>0.2243893377913997</v>
       </c>
     </row>
     <row r="58">
@@ -1473,7 +1473,7 @@
         </is>
       </c>
       <c r="D58" t="n">
-        <v>3.363</v>
+        <v>0.239899693507941</v>
       </c>
     </row>
     <row r="59">
@@ -1491,7 +1491,7 @@
         </is>
       </c>
       <c r="D59" t="n">
-        <v>1.476</v>
+        <v>0</v>
       </c>
     </row>
     <row r="60">
@@ -1509,7 +1509,7 @@
         </is>
       </c>
       <c r="D60" t="n">
-        <v>3.344</v>
+        <v>0.4667966936008173</v>
       </c>
     </row>
     <row r="61">
@@ -1545,7 +1545,7 @@
         </is>
       </c>
       <c r="D62" t="n">
-        <v>2.29617592893511</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63">
@@ -1563,7 +1563,7 @@
         </is>
       </c>
       <c r="D63" t="n">
-        <v>4.836</v>
+        <v>0.2128726664809139</v>
       </c>
     </row>
     <row r="64">
@@ -1581,7 +1581,7 @@
         </is>
       </c>
       <c r="D64" t="n">
-        <v>3.45</v>
+        <v>0.4276957369740875</v>
       </c>
     </row>
     <row r="65">
@@ -1599,7 +1599,7 @@
         </is>
       </c>
       <c r="D65" t="n">
-        <v>2.098</v>
+        <v>0.2890312993405777</v>
       </c>
     </row>
     <row r="66">
@@ -1617,7 +1617,7 @@
         </is>
       </c>
       <c r="D66" t="n">
-        <v>6.65</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67">
@@ -1635,7 +1635,7 @@
         </is>
       </c>
       <c r="D67" t="n">
-        <v>1.766507287768367</v>
+        <v>0</v>
       </c>
     </row>
     <row r="68">
@@ -1653,7 +1653,7 @@
         </is>
       </c>
       <c r="D68" t="n">
-        <v>1.993</v>
+        <v>0.1637410606482771</v>
       </c>
     </row>
     <row r="69">
@@ -1671,7 +1671,7 @@
         </is>
       </c>
       <c r="D69" t="n">
-        <v>3.095</v>
+        <v>0.1525958948639361</v>
       </c>
     </row>
     <row r="70">
@@ -1689,7 +1689,7 @@
         </is>
       </c>
       <c r="D70" t="n">
-        <v>2.00708627142013</v>
+        <v>0</v>
       </c>
     </row>
     <row r="71">
@@ -1707,7 +1707,7 @@
         </is>
       </c>
       <c r="D71" t="n">
-        <v>3.822</v>
+        <v>0.1861242685984954</v>
       </c>
     </row>
     <row r="72">
@@ -1725,7 +1725,7 @@
         </is>
       </c>
       <c r="D72" t="n">
-        <v>5.223</v>
+        <v>0.7430110522894029</v>
       </c>
     </row>
     <row r="73">
@@ -1743,7 +1743,7 @@
         </is>
       </c>
       <c r="D73" t="n">
-        <v>4.012</v>
+        <v>0.5112844803566453</v>
       </c>
     </row>
     <row r="74">
@@ -1761,7 +1761,7 @@
         </is>
       </c>
       <c r="D74" t="n">
-        <v>2.195</v>
+        <v>0.08386737252716635</v>
       </c>
     </row>
     <row r="75">
@@ -1797,7 +1797,7 @@
         </is>
       </c>
       <c r="D76" t="n">
-        <v>0.919</v>
+        <v>0</v>
       </c>
     </row>
     <row r="77">
@@ -1815,7 +1815,7 @@
         </is>
       </c>
       <c r="D77" t="n">
-        <v>0.757</v>
+        <v>0.1206464196154918</v>
       </c>
     </row>
     <row r="78">
@@ -1833,7 +1833,7 @@
         </is>
       </c>
       <c r="D78" t="n">
-        <v>7.84</v>
+        <v>0.8964428345871644</v>
       </c>
     </row>
     <row r="79">
@@ -1851,7 +1851,7 @@
         </is>
       </c>
       <c r="D79" t="n">
-        <v>2.839</v>
+        <v>0.1292839230983561</v>
       </c>
     </row>
     <row r="80">
@@ -1869,7 +1869,7 @@
         </is>
       </c>
       <c r="D80" t="n">
-        <v>3.353</v>
+        <v>0.2642333054704189</v>
       </c>
     </row>
     <row r="81">
@@ -1887,7 +1887,7 @@
         </is>
       </c>
       <c r="D81" t="n">
-        <v>1.454</v>
+        <v>0.1674561159097241</v>
       </c>
     </row>
     <row r="82">
@@ -1905,7 +1905,7 @@
         </is>
       </c>
       <c r="D82" t="n">
-        <v>4.696769745912941</v>
+        <v>0</v>
       </c>
     </row>
     <row r="83">
@@ -1923,7 +1923,7 @@
         </is>
       </c>
       <c r="D83" t="n">
-        <v>2.743</v>
+        <v>0.4392124082845733</v>
       </c>
     </row>
   </sheetData>

</xml_diff>